<commit_message>
SOlved issue with computing relative excess deaths
</commit_message>
<xml_diff>
--- a/paper/Table_2.xlsx
+++ b/paper/Table_2.xlsx
@@ -26,18 +26,18 @@
     <t xml:space="preserve">excess_cri</t>
   </si>
   <si>
+    <t xml:space="preserve">Rate_excess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_cri</t>
+  </si>
+  <si>
     <t xml:space="preserve">Percent_excess</t>
   </si>
   <si>
     <t xml:space="preserve">percent_cri</t>
   </si>
   <si>
-    <t xml:space="preserve">Rate_excess</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_cri</t>
-  </si>
-  <si>
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
@@ -47,18 +47,18 @@
     <t xml:space="preserve">(663; 6,135)</t>
   </si>
   <si>
+    <t xml:space="preserve">115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20; 210)</t>
+  </si>
+  <si>
     <t xml:space="preserve">5.9%</t>
   </si>
   <si>
     <t xml:space="preserve">(1.1%; 10.5%)</t>
   </si>
   <si>
-    <t xml:space="preserve">115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20; 210)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
@@ -68,54 +68,54 @@
     <t xml:space="preserve">(4,875; 12,512)</t>
   </si>
   <si>
+    <t xml:space="preserve">185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(100; 260)</t>
+  </si>
+  <si>
     <t xml:space="preserve">12.0%</t>
   </si>
   <si>
     <t xml:space="preserve">(6.7%; 17.1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(100; 260)</t>
-  </si>
-  <si>
     <t xml:space="preserve">24,697</t>
   </si>
   <si>
     <t xml:space="preserve">(21,881; 27,487)</t>
   </si>
   <si>
+    <t xml:space="preserve">635</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(565; 710)</t>
+  </si>
+  <si>
     <t xml:space="preserve">49.1%</t>
   </si>
   <si>
     <t xml:space="preserve">(43.5%; 54.6%)</t>
   </si>
   <si>
-    <t xml:space="preserve">635</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(565; 710)</t>
-  </si>
-  <si>
     <t xml:space="preserve">25,894</t>
   </si>
   <si>
     <t xml:space="preserve">(20,635; 31,002)</t>
   </si>
   <si>
+    <t xml:space="preserve">445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(355; 535)</t>
+  </si>
+  <si>
     <t xml:space="preserve">32.9%</t>
   </si>
   <si>
     <t xml:space="preserve">(26.2%; 39.4%)</t>
   </si>
   <si>
-    <t xml:space="preserve">445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(355; 535)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
@@ -125,157 +125,157 @@
     <t xml:space="preserve">(216,478; 266,104)</t>
   </si>
   <si>
+    <t xml:space="preserve">1,135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1,015; 1,250)</t>
+  </si>
+  <si>
     <t xml:space="preserve">53.3%</t>
   </si>
   <si>
     <t xml:space="preserve">(47.7%; 58.6%)</t>
   </si>
   <si>
-    <t xml:space="preserve">1,135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,015; 1,250)</t>
-  </si>
-  <si>
     <t xml:space="preserve">-929</t>
   </si>
   <si>
     <t xml:space="preserve">(-3,725; 1,789)</t>
   </si>
   <si>
+    <t xml:space="preserve">-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-75; 35)</t>
+  </si>
+  <si>
     <t xml:space="preserve">-1.8%</t>
   </si>
   <si>
     <t xml:space="preserve">(-7.2%; 3.4%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-75; 35)</t>
-  </si>
-  <si>
     <t xml:space="preserve">2,745</t>
   </si>
   <si>
     <t xml:space="preserve">(138; 5,338)</t>
   </si>
   <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0; 75)</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.9%</t>
   </si>
   <si>
     <t xml:space="preserve">(0.2%; 7.6%)</t>
   </si>
   <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0; 75)</t>
-  </si>
-  <si>
     <t xml:space="preserve">13,585</t>
   </si>
   <si>
     <t xml:space="preserve">(-2,296; 29,062)</t>
   </si>
   <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-10; 100)</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.9%</t>
   </si>
   <si>
     <t xml:space="preserve">(-0.8%; 10.4%)</t>
   </si>
   <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-10; 100)</t>
-  </si>
-  <si>
     <t xml:space="preserve">8,478</t>
   </si>
   <si>
     <t xml:space="preserve">(5,336; 11,494)</t>
   </si>
   <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(60; 135)</t>
+  </si>
+  <si>
     <t xml:space="preserve">12.5%</t>
   </si>
   <si>
     <t xml:space="preserve">(7.9%; 17.0%)</t>
   </si>
   <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(60; 135)</t>
-  </si>
-  <si>
     <t xml:space="preserve">7,664</t>
   </si>
   <si>
     <t xml:space="preserve">(4,234; 11,015)</t>
   </si>
   <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(40; 105)</t>
+  </si>
+  <si>
     <t xml:space="preserve">8.5%</t>
   </si>
   <si>
     <t xml:space="preserve">(4.7%; 12.2%)</t>
   </si>
   <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(40; 105)</t>
-  </si>
-  <si>
     <t xml:space="preserve">71,917</t>
   </si>
   <si>
     <t xml:space="preserve">(51,869; 91,809)</t>
   </si>
   <si>
+    <t xml:space="preserve">150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(110; 195)</t>
+  </si>
+  <si>
     <t xml:space="preserve">17.1%</t>
   </si>
   <si>
     <t xml:space="preserve">(12.3%; 21.8%)</t>
   </si>
   <si>
-    <t xml:space="preserve">150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(110; 195)</t>
-  </si>
-  <si>
     <t xml:space="preserve">-998</t>
   </si>
   <si>
     <t xml:space="preserve">(-3,040; 957)</t>
   </si>
   <si>
+    <t xml:space="preserve">-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-35; 10)</t>
+  </si>
+  <si>
     <t xml:space="preserve">-2.8%</t>
   </si>
   <si>
     <t xml:space="preserve">(-8.5%; 2.7%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-35; 10)</t>
-  </si>
-  <si>
     <t xml:space="preserve">10,950</t>
   </si>
   <si>
     <t xml:space="preserve">(-3,300; 24,187)</t>
   </si>
   <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-5; 50)</t>
+  </si>
+  <si>
     <t xml:space="preserve">(-1.5%; 10.8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5; 50)</t>
   </si>
 </sst>
 </file>
@@ -973,13 +973,13 @@
         <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="H15" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
outputs from new results
cleaning up data reads, variable names, still with multiple versions of figures
</commit_message>
<xml_diff>
--- a/paper/Table_2.xlsx
+++ b/paper/Table_2.xlsx
@@ -263,10 +263,10 @@
     <t xml:space="preserve">(-8.2%; 2.8%)</t>
   </si>
   <si>
-    <t xml:space="preserve">10,836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,459; 24,437)</t>
+    <t xml:space="preserve">10,867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3,423; 24,715)</t>
   </si>
   <si>
     <t xml:space="preserve">25</t>
@@ -275,10 +275,10 @@
     <t xml:space="preserve">(-5; 50)</t>
   </si>
   <si>
-    <t xml:space="preserve">4.9%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1.5%; 11.6%)</t>
+    <t xml:space="preserve">5.0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1.4%; 11.8%)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
reshuffling content, fixing names, update of outputs
</commit_message>
<xml_diff>
--- a/paper/Table_2.xlsx
+++ b/paper/Table_2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -38,6 +38,9 @@
     <t xml:space="preserve">percent_cri</t>
   </si>
   <si>
+    <t xml:space="preserve">Lifeyearlost70_CI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t xml:space="preserve">(1.2%; 11.0%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-38 to 136</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
@@ -80,6 +86,9 @@
     <t xml:space="preserve">(6.3%; 18.2%)</t>
   </si>
   <si>
+    <t xml:space="preserve">109 to 361</t>
+  </si>
+  <si>
     <t xml:space="preserve">24,730</t>
   </si>
   <si>
@@ -98,6 +107,9 @@
     <t xml:space="preserve">(41.3%; 57.7%)</t>
   </si>
   <si>
+    <t xml:space="preserve">834 to 965</t>
+  </si>
+  <si>
     <t xml:space="preserve">25,937</t>
   </si>
   <si>
@@ -116,6 +128,9 @@
     <t xml:space="preserve">(24.5%; 42.3%)</t>
   </si>
   <si>
+    <t xml:space="preserve">945 to 1189</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
@@ -137,6 +152,9 @@
     <t xml:space="preserve">(45.0%; 61.9%)</t>
   </si>
   <si>
+    <t xml:space="preserve">9132 to 10926</t>
+  </si>
+  <si>
     <t xml:space="preserve">-922</t>
   </si>
   <si>
@@ -155,6 +173,9 @@
     <t xml:space="preserve">(-6.7%; 3.7%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-51 to 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">2,760</t>
   </si>
   <si>
@@ -173,6 +194,9 @@
     <t xml:space="preserve">(0.1%; 7.9%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-13 to 30</t>
+  </si>
+  <si>
     <t xml:space="preserve">13,227</t>
   </si>
   <si>
@@ -191,6 +215,9 @@
     <t xml:space="preserve">(-0.9%; 10.9%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-383 to 172</t>
+  </si>
+  <si>
     <t xml:space="preserve">8,429</t>
   </si>
   <si>
@@ -209,6 +236,9 @@
     <t xml:space="preserve">(7.4%; 17.7%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-3 to 15</t>
+  </si>
+  <si>
     <t xml:space="preserve">7,656</t>
   </si>
   <si>
@@ -227,6 +257,9 @@
     <t xml:space="preserve">(4.5%; 12.6%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-6 to 13</t>
+  </si>
+  <si>
     <t xml:space="preserve">72,328</t>
   </si>
   <si>
@@ -245,6 +278,9 @@
     <t xml:space="preserve">(11.8%; 23.1%)</t>
   </si>
   <si>
+    <t xml:space="preserve">39 to 145</t>
+  </si>
+  <si>
     <t xml:space="preserve">-1,002</t>
   </si>
   <si>
@@ -263,6 +299,9 @@
     <t xml:space="preserve">(-8.2%; 2.8%)</t>
   </si>
   <si>
+    <t xml:space="preserve">-12 to 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">10,867</t>
   </si>
   <si>
@@ -279,6 +318,9 @@
   </si>
   <si>
     <t xml:space="preserve">(-1.4%; 11.8%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-32 to 41</t>
   </si>
 </sst>
 </file>
@@ -635,31 +677,37 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1890</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -667,25 +715,28 @@
         <v>1890</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -693,25 +744,28 @@
         <v>1918</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -719,25 +773,28 @@
         <v>1918</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6">
@@ -745,25 +802,28 @@
         <v>1918</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="7">
@@ -771,25 +831,28 @@
         <v>1957</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8">
@@ -797,25 +860,28 @@
         <v>1957</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -823,25 +889,28 @@
         <v>1957</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
+        <v>66</v>
+      </c>
+      <c r="I9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10">
@@ -849,25 +918,28 @@
         <v>2020</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11">
@@ -875,25 +947,28 @@
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="I11" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12">
@@ -901,25 +976,28 @@
         <v>2020</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13">
@@ -927,25 +1005,28 @@
         <v>2021</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="I13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="14">
@@ -953,7 +1034,7 @@
         <v>2021</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -961,31 +1042,35 @@
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
+      <c r="I14"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G15" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>101</v>
+      </c>
+      <c r="I15" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reknit check before 2.1 release
</commit_message>
<xml_diff>
--- a/paper/Table_2.xlsx
+++ b/paper/Table_2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -65,10 +65,10 @@
     <t xml:space="preserve">(1.2% to 11.0%)</t>
   </si>
   <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-40 to 135)</t>
+    <t xml:space="preserve">7,740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6,000 to 21,190)</t>
   </si>
   <si>
     <t xml:space="preserve">Sweden</t>
@@ -92,10 +92,10 @@
     <t xml:space="preserve">(6.3% to 18.2%)</t>
   </si>
   <si>
-    <t xml:space="preserve">235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(110 to 360)</t>
+    <t xml:space="preserve">21,405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(9,825 to 32,595)</t>
   </si>
   <si>
     <t xml:space="preserve">24,730</t>
@@ -116,10 +116,10 @@
     <t xml:space="preserve">(41.3% to 57.7%)</t>
   </si>
   <si>
-    <t xml:space="preserve">900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(835 to 965)</t>
+    <t xml:space="preserve">120,895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(112,000 to 129,665)</t>
   </si>
   <si>
     <t xml:space="preserve">25,937</t>
@@ -140,10 +140,10 @@
     <t xml:space="preserve">(24.5% to 42.3%)</t>
   </si>
   <si>
-    <t xml:space="preserve">1,070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(945 to 1,190)</t>
+    <t xml:space="preserve">91,090</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(80,630 to 101,400)</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
@@ -167,10 +167,10 @@
     <t xml:space="preserve">(45.0% to 61.9%)</t>
   </si>
   <si>
-    <t xml:space="preserve">10,050</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(9,130 to 10,925)</t>
+    <t xml:space="preserve">210,070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(190,845 to 228,345)</t>
   </si>
   <si>
     <t xml:space="preserve">-922</t>
@@ -191,7 +191,10 @@
     <t xml:space="preserve">(-6.7% to 3.7%)</t>
   </si>
   <si>
-    <t xml:space="preserve">(-50 to 5)</t>
+    <t xml:space="preserve">-2,650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6,030 to 730)</t>
   </si>
   <si>
     <t xml:space="preserve">2,760</t>
@@ -212,10 +215,10 @@
     <t xml:space="preserve">(0.1% to 7.9%)</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-15 to 30)</t>
+    <t xml:space="preserve">775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,155 to 2,680)</t>
   </si>
   <si>
     <t xml:space="preserve">13,227</t>
@@ -236,10 +239,10 @@
     <t xml:space="preserve">(-0.9% to 10.9%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-385 to 170)</t>
+    <t xml:space="preserve">-1,900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-7,055 to 3,180)</t>
   </si>
   <si>
     <t xml:space="preserve">8,429</t>
@@ -260,10 +263,10 @@
     <t xml:space="preserve">(7.4% to 17.7%)</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-5 to 15)</t>
+    <t xml:space="preserve">695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-400 to 1,760)</t>
   </si>
   <si>
     <t xml:space="preserve">7,656</t>
@@ -284,6 +287,12 @@
     <t xml:space="preserve">(4.5% to 12.6%)</t>
   </si>
   <si>
+    <t xml:space="preserve">260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-520 to 1,030)</t>
+  </si>
+  <si>
     <t xml:space="preserve">72,328</t>
   </si>
   <si>
@@ -302,10 +311,10 @@
     <t xml:space="preserve">(11.8% to 23.1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(40 to 145)</t>
+    <t xml:space="preserve">2,130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(900 to 3,335)</t>
   </si>
   <si>
     <t xml:space="preserve">-1,002</t>
@@ -326,10 +335,10 @@
     <t xml:space="preserve">(-8.2% to 2.8%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-10 to 0)</t>
+    <t xml:space="preserve">-625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1,335 to 85)</t>
   </si>
   <si>
     <t xml:space="preserve">10,867</t>
@@ -350,7 +359,7 @@
     <t xml:space="preserve">(-1.4% to 11.8%)</t>
   </si>
   <si>
-    <t xml:space="preserve">(-30 to 40)</t>
+    <t xml:space="preserve">(-770 to 975)</t>
   </si>
 </sst>
 </file>
@@ -900,10 +909,10 @@
         <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
@@ -914,28 +923,28 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
@@ -946,28 +955,28 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10">
@@ -978,28 +987,28 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
@@ -1010,28 +1019,28 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12">
@@ -1042,28 +1051,28 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -1074,28 +1083,28 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I13" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="J13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
@@ -1122,28 +1131,28 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F15" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
table2 with journal's edits
</commit_message>
<xml_diff>
--- a/paper/Table_2.xlsx
+++ b/paper/Table_2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -38,19 +38,13 @@
     <t xml:space="preserve">percent_cri</t>
   </si>
   <si>
-    <t xml:space="preserve">Lifeyearlost70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lifeyearlost70_CI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Switzerland</t>
   </si>
   <si>
-    <t xml:space="preserve">3,456</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(703 to 6,118)</t>
+    <t xml:space="preserve">3 456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(703 to 6 118)</t>
   </si>
   <si>
     <t xml:space="preserve">115</t>
@@ -59,25 +53,19 @@
     <t xml:space="preserve">(25 to 205)</t>
   </si>
   <si>
-    <t xml:space="preserve">6.0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1.2% to 11.0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,740</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,000 to 21,190)</t>
+    <t xml:space="preserve">6.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1.2 to 11.0)</t>
   </si>
   <si>
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
-    <t xml:space="preserve">8,810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,871 to 12,573)</t>
+    <t xml:space="preserve">8 810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 871 to 12 573)</t>
   </si>
   <si>
     <t xml:space="preserve">185</t>
@@ -86,22 +74,16 @@
     <t xml:space="preserve">(100 to 265)</t>
   </si>
   <si>
-    <t xml:space="preserve">12.1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(6.3% to 18.2%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(9,825 to 32,595)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24,730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(21,925 to 27,453)</t>
+    <t xml:space="preserve">12.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(6.3 to 18.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(21 925 to 27 453)</t>
   </si>
   <si>
     <t xml:space="preserve">640</t>
@@ -110,22 +92,16 @@
     <t xml:space="preserve">(565 to 710)</t>
   </si>
   <si>
-    <t xml:space="preserve">49.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(41.3% to 57.7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120,895</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(112,000 to 129,665)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,937</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(20,597 to 31,087)</t>
+    <t xml:space="preserve">49.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(41.3 to 57.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(20 597 to 31 087)</t>
   </si>
   <si>
     <t xml:space="preserve">445</t>
@@ -134,49 +110,37 @@
     <t xml:space="preserve">(355 to 535)</t>
   </si>
   <si>
-    <t xml:space="preserve">33.1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(24.5% to 42.3%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91,090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(80,630 to 101,400)</t>
+    <t xml:space="preserve">33.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(24.5 to 42.3)</t>
   </si>
   <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">241,661</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(215,791 to 266,103)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1,015 to 1,250)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(45.0% to 61.9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">210,070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(190,845 to 228,345)</t>
+    <t xml:space="preserve">241 661</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(215 791 to 266 103)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1 015 to 1 250)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(45.0 to 61.9)</t>
   </si>
   <si>
     <t xml:space="preserve">-922</t>
   </si>
   <si>
-    <t xml:space="preserve">(-3,679 to 1,804)</t>
+    <t xml:space="preserve">(-3 679 to 1 804)</t>
   </si>
   <si>
     <t xml:space="preserve">-20</t>
@@ -185,22 +149,16 @@
     <t xml:space="preserve">(-70 to 35)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6.7% to 3.7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2,650</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-6,030 to 730)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,760</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(101 to 5,338)</t>
+    <t xml:space="preserve">-1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-6.7 to 3.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(101 to 5 338)</t>
   </si>
   <si>
     <t xml:space="preserve">40</t>
@@ -209,22 +167,16 @@
     <t xml:space="preserve">(0 to 75)</t>
   </si>
   <si>
-    <t xml:space="preserve">4.0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(0.1% to 7.9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">775</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,155 to 2,680)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,227</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-2,659 to 28,783)</t>
+    <t xml:space="preserve">4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0.1 to 7.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-2 659 to 28 783)</t>
   </si>
   <si>
     <t xml:space="preserve">45</t>
@@ -233,22 +185,16 @@
     <t xml:space="preserve">(-10 to 100)</t>
   </si>
   <si>
-    <t xml:space="preserve">4.8%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-0.9% to 10.9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,900</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-7,055 to 3,180)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8,429</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(5,253 to 11,449)</t>
+    <t xml:space="preserve">4.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-0.9 to 10.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(5 253 to 11 449)</t>
   </si>
   <si>
     <t xml:space="preserve">100</t>
@@ -257,22 +203,16 @@
     <t xml:space="preserve">(60 to 135)</t>
   </si>
   <si>
-    <t xml:space="preserve">12.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(7.4% to 17.7%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">695</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-400 to 1,760)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,656</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4,199 to 10,984)</t>
+    <t xml:space="preserve">12.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(7.4 to 17.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 656</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4 199 to 10 984)</t>
   </si>
   <si>
     <t xml:space="preserve">75</t>
@@ -281,22 +221,16 @@
     <t xml:space="preserve">(40 to 105)</t>
   </si>
   <si>
-    <t xml:space="preserve">8.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(4.5% to 12.6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-520 to 1,030)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72,328</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(51,942 to 92,409)</t>
+    <t xml:space="preserve">8.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4.5 to 12.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72 328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(51 942 to 92 409)</t>
   </si>
   <si>
     <t xml:space="preserve">155</t>
@@ -305,22 +239,16 @@
     <t xml:space="preserve">(110 to 195)</t>
   </si>
   <si>
-    <t xml:space="preserve">17.3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(11.8% to 23.1%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(900 to 3,335)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,087 to 957)</t>
+    <t xml:space="preserve">17.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(11.8 to 23.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1 002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 087 to 957)</t>
   </si>
   <si>
     <t xml:space="preserve">-10</t>
@@ -329,22 +257,16 @@
     <t xml:space="preserve">(-35 to 10)</t>
   </si>
   <si>
-    <t xml:space="preserve">-2.7%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-8.2% to 2.8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1,335 to 85)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,867</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-3,423 to 24,715)</t>
+    <t xml:space="preserve">-2.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-8.2 to 2.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-3 423 to 24 715)</t>
   </si>
   <si>
     <t xml:space="preserve">25</t>
@@ -353,13 +275,10 @@
     <t xml:space="preserve">(-5 to 50)</t>
   </si>
   <si>
-    <t xml:space="preserve">5.0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-1.4% to 11.8%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(-770 to 975)</t>
+    <t xml:space="preserve">5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(-1.4 to 11.8)</t>
   </si>
 </sst>
 </file>
@@ -716,43 +635,31 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1890</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -760,31 +667,25 @@
         <v>1890</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -792,31 +693,25 @@
         <v>1918</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -824,31 +719,25 @@
         <v>1918</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -856,31 +745,25 @@
         <v>1918</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -888,31 +771,25 @@
         <v>1957</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
@@ -920,31 +797,25 @@
         <v>1957</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" t="s">
-        <v>67</v>
-      </c>
-      <c r="J8" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
@@ -952,31 +823,25 @@
         <v>1957</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10">
@@ -984,31 +849,25 @@
         <v>2020</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="H10" t="s">
-        <v>82</v>
-      </c>
-      <c r="I10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J10" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
@@ -1016,31 +875,25 @@
         <v>2020</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
-      </c>
-      <c r="I11" t="s">
-        <v>91</v>
-      </c>
-      <c r="J11" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
@@ -1048,31 +901,25 @@
         <v>2020</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>98</v>
-      </c>
-      <c r="I12" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -1080,31 +927,25 @@
         <v>2021</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J13" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
@@ -1112,7 +953,7 @@
         <v>2021</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -1120,39 +961,31 @@
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>2021</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
-      </c>
-      <c r="I15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>